<commit_message>
Update NextGen Member of BBS Board
</commit_message>
<xml_diff>
--- a/data/roster.xlsx
+++ b/data/roster.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10608"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\rufibach\70_Service\BBS\webpage\home\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/widmelu1/Documents/git/bbs-basel/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B647142-B909-4AAE-BBB6-FE89DF274460}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C76712A-E3B6-124C-9952-32CF8E1FFA09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="77820" yWindow="4260" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2020 Roster" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="94">
   <si>
     <t>Kaspar</t>
   </si>
@@ -276,15 +276,6 @@
     <t>UCB</t>
   </si>
   <si>
-    <t>YouYou</t>
-  </si>
-  <si>
-    <t>Hu</t>
-  </si>
-  <si>
-    <t>youyou.hu@roche.com</t>
-  </si>
-  <si>
     <t>NextGen representative</t>
   </si>
   <si>
@@ -307,6 +298,18 @@
   </si>
   <si>
     <t>Weber</t>
+  </si>
+  <si>
+    <t>Ottavia</t>
+  </si>
+  <si>
+    <t>Prunas</t>
+  </si>
+  <si>
+    <t>ottavia.prunas@unibas.ch</t>
+  </si>
+  <si>
+    <t>University Hospital of Basel</t>
   </si>
 </sst>
 </file>
@@ -374,8 +377,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -691,23 +694,23 @@
   <dimension ref="A1:T25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="101.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="101.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="100.85546875" style="2" customWidth="1"/>
-    <col min="8" max="20" width="101.5703125" style="2"/>
-    <col min="21" max="16384" width="101.5703125" style="1"/>
+    <col min="1" max="1" width="10.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="100.83203125" style="2" customWidth="1"/>
+    <col min="8" max="20" width="101.5" style="2"/>
+    <col min="21" max="16384" width="101.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>57</v>
       </c>
@@ -730,7 +733,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
@@ -747,7 +750,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
@@ -764,7 +767,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -784,7 +787,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>23</v>
       </c>
@@ -801,7 +804,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>31</v>
       </c>
@@ -821,7 +824,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
@@ -838,7 +841,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
@@ -855,7 +858,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -875,7 +878,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>27</v>
       </c>
@@ -895,7 +898,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>5</v>
       </c>
@@ -912,7 +915,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
@@ -929,7 +932,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -943,7 +946,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>29</v>
       </c>
@@ -960,7 +963,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>21</v>
       </c>
@@ -977,7 +980,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>43</v>
       </c>
@@ -995,7 +998,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>54</v>
       </c>
@@ -1015,7 +1018,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>60</v>
       </c>
@@ -1032,7 +1035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>62</v>
       </c>
@@ -1049,7 +1052,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>68</v>
       </c>
@@ -1066,7 +1069,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>71</v>
       </c>
@@ -1083,32 +1086,32 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" ht="16" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="E22" s="2">
+        <v>1</v>
+      </c>
+      <c r="G22" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B22" s="1" t="s">
+    </row>
+    <row r="23" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D22" s="5" t="s">
+      <c r="B23" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="E22" s="2">
-        <v>1</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>87</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>81</v>
@@ -1117,26 +1120,26 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E24" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B25" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E24" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>92</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>33</v>

</xml_diff>